<commit_message>
Successfully implemented search logic in server.js
</commit_message>
<xml_diff>
--- a/src/excelfiles/praythisworksv2.xlsx
+++ b/src/excelfiles/praythisworksv2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tisea\spcpwebpage\spcpdbwebpage\src\excelfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21FDCD6-3A51-4BF9-8D9A-BF0AD00B770B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48129CA8-994F-4B5F-8BD1-D6CFE892C532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4DE437C2-E894-4E62-8CB9-3ED00E505C4C}"/>
   </bookViews>
@@ -15860,8 +15860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADA3DC1-39D5-4707-B2A2-3745524CD2B7}">
   <dimension ref="A1:G225"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D203" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20874,7 +20874,7 @@
         <v>0.17590063970670758</v>
       </c>
       <c r="E213" s="4">
-        <f t="shared" si="14"/>
+        <f>E189/E$179</f>
         <v>0.20923520923520925</v>
       </c>
       <c r="F213" s="4">
@@ -21268,7 +21268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B684874-516B-4063-9A51-DCFC2DA3ED08}">
   <dimension ref="A1:N283"/>
   <sheetViews>
-    <sheetView zoomScale="51" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="51" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D260" sqref="D260"/>
     </sheetView>
   </sheetViews>

</xml_diff>